<commit_message>
code review + příprava pro změny VHL
</commit_message>
<xml_diff>
--- a/data/03_zpracovano/PPP_archivZpracovanychPolozek.xlsx
+++ b/data/03_zpracovano/PPP_archivZpracovanychPolozek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlava\Documents\UiPath\PPP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hladilpet\Documents\UiPath\PPP_final\data\03_zpracovano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AE9112-6A0E-46AD-AEB9-433537AA005B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915D6AF3-A41E-48E7-A45C-F5CE585E75D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-210" yWindow="16080" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34890" yWindow="90" windowWidth="18180" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPA-zpracovano" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="212">
   <si>
     <t>No.</t>
   </si>
@@ -145,6 +142,700 @@
   </si>
   <si>
     <t>Robot - datum poslední aktualizace</t>
+  </si>
+  <si>
+    <t>Dzurik Ondřej</t>
+  </si>
+  <si>
+    <t>859182400705251092</t>
+  </si>
+  <si>
+    <t>MZS</t>
+  </si>
+  <si>
+    <t>VČE Východočeská energetika</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>QPSDVYCHOD</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 24.2.2021. EAN 859182400705251092. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Čez Prodej</t>
+  </si>
+  <si>
+    <t>zmena.dodavatele@cez.cz</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400705251092</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400705251092 - Josef Emlar/15.03.1943, Hořenice, 15, Hořenice, 551 01.
+Montáž 4Q elektroměru bude 24.02.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D25D, Pi 4,44 kW, HDO ANO, KO č. 1113392241 , Josef Emlar, 608370855</t>
+  </si>
+  <si>
+    <t>DZURIKOND</t>
+  </si>
+  <si>
+    <t>Josef Emlar</t>
+  </si>
+  <si>
+    <t>Hořenice, 15, Hořenice, 551 01</t>
+  </si>
+  <si>
+    <t>15.03.1943</t>
+  </si>
+  <si>
+    <t>25,0</t>
+  </si>
+  <si>
+    <t>PE8D25D</t>
+  </si>
+  <si>
+    <t>proces3: Success</t>
+  </si>
+  <si>
+    <t>24.02.2021 10:02</t>
+  </si>
+  <si>
+    <t>859182400705251093</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 24.2.2021. EAN 859182400705251093. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400705251093</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400705251093 - Josef Emlar/15.03.1943, Hořenice, 15, Hořenice, 551 01.
+Montáž 4Q elektroměru bude 24.02.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>proces3: zpracováno</t>
+  </si>
+  <si>
+    <t>24.02.2021 10:03</t>
+  </si>
+  <si>
+    <t>859182400705251094</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 24.2.2021. EAN 859182400705251094. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400705251094</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400705251094 - Josef Emlar/15.03.1943, Hořenice, 15, Hořenice, 551 01.
+Montáž 4Q elektroměru bude 24.02.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>26.02.2021 01:07</t>
+  </si>
+  <si>
+    <t>26.02.2021 01:15</t>
+  </si>
+  <si>
+    <t>859182400408602337</t>
+  </si>
+  <si>
+    <t>SČE Severočeská energetika</t>
+  </si>
+  <si>
+    <t>QPSDSEVER</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 22.3.2021. EAN 859182400408602337. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>vyrobny@cez.cz</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400408602337</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400408602337 - David Odstrčil/12.09.1979, Dr. Václava Kůrky, 2830, Žatec, 438 01.
+Montáž 4Q elektroměru bude 22.03.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D57D, Pi 4,4 kW, HDO ANO, KO č. 1113074378 , David Odstrčil, 775155495</t>
+  </si>
+  <si>
+    <t>David Odstrčil</t>
+  </si>
+  <si>
+    <t>Dr. Václava Kůrky, 2830, Žatec, 438 01</t>
+  </si>
+  <si>
+    <t>12.09.1979</t>
+  </si>
+  <si>
+    <t>PE8D57D</t>
+  </si>
+  <si>
+    <t>12.03.2021 01:05</t>
+  </si>
+  <si>
+    <t>859182400601566726</t>
+  </si>
+  <si>
+    <t>STE Středočeská energetika</t>
+  </si>
+  <si>
+    <t>QPSDSTRED</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 22.3.2021. EAN 859182400601566726. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>E. ON Energie, a.s.</t>
+  </si>
+  <si>
+    <t>DM@eon.cz</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400601566726</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400601566726 - Jana Knorová/29.10.1957, Jelení, 2123, Říčany, 251 01.
+Montáž 4Q elektroměru bude 22.03.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D02D, Pi 8,25 kW, HDO ANO, KO č. 1114184179 , Jana Knorová, 739306042</t>
+  </si>
+  <si>
+    <t>Jana Knorová</t>
+  </si>
+  <si>
+    <t>Jelení, 2123, Říčany, 251 01</t>
+  </si>
+  <si>
+    <t>29.10.1957</t>
+  </si>
+  <si>
+    <t>PE8D02D</t>
+  </si>
+  <si>
+    <t>12.03.2021 01:19</t>
+  </si>
+  <si>
+    <t>859182400707101241</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 20.4.2021. EAN 859182400707101241. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400707101241</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400707101241 - Daniel Chymo/01.03.1975, Poděbaby, 159, Havlíčkův Brod, 580 01.
+Montáž 4Q elektroměru bude 20.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 32,0 A, sazba D56D, Pi 5,52 kW, HDO ANO, KO č. 1114734978 , Daniel Chymo, 775077382</t>
+  </si>
+  <si>
+    <t>Daniel Chymo</t>
+  </si>
+  <si>
+    <t>Poděbaby, 159, Havlíčkův Brod, 580 01</t>
+  </si>
+  <si>
+    <t>01.03.1975</t>
+  </si>
+  <si>
+    <t>32,0</t>
+  </si>
+  <si>
+    <t>PE8D56D</t>
+  </si>
+  <si>
+    <t>09.04.2021 11:40</t>
+  </si>
+  <si>
+    <t>859182400506904005</t>
+  </si>
+  <si>
+    <t>SME Severomoravská Energetika</t>
+  </si>
+  <si>
+    <t>QPSDMORAVA</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 16.4.2021. EAN 859182400506904005. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400506904005</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400506904005 - Hynek Olchava/10.10.1976, Na Janošku, 578, Ostrava-Hrabová, 720 00.
+Montáž 4Q elektroměru bude 16.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D02D, Pi 2,58 kW, HDO ANO, KO č. 1114733390 , Hynek Olchava, 739054589</t>
+  </si>
+  <si>
+    <t>Hynek Olchava</t>
+  </si>
+  <si>
+    <t>Na Janošku, 578, Ostrava-Hrabová, 720 00</t>
+  </si>
+  <si>
+    <t>10.10.1976</t>
+  </si>
+  <si>
+    <t>09.04.2021 11:51</t>
+  </si>
+  <si>
+    <t>Gryžboň Jakub</t>
+  </si>
+  <si>
+    <t>859182400605584139</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 20.4.2021. EAN 859182400605584139. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Europe Easy Energy a.s.</t>
+  </si>
+  <si>
+    <t>zmena.dodavatele@3-e.cz;distribucnipozadavky@3-e.cz</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400605584139</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400605584139 - Jaroslav Hroník/[12:52] Dzurik Ondřej
+    04.08.1960, Želízy 85, 277 21 Želízy.
+Montáž 4Q elektroměru bude 20.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Gryžboň Jakub
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 3x25 A, sazba D25D, Pi 0,00462 kW, HDO ANO, KO č. 1114769081 , Jaroslav Hroník, 603432156</t>
+  </si>
+  <si>
+    <t>GRYZBONJAK</t>
+  </si>
+  <si>
+    <t>Jaroslav Hroník</t>
+  </si>
+  <si>
+    <t>Želízy 85, 277 21 Želízy</t>
+  </si>
+  <si>
+    <t>[12:52] Dzurik Ondřej
+    04.08.1960</t>
+  </si>
+  <si>
+    <t>[12:52] Dzurik Ondřej
+11242264</t>
+  </si>
+  <si>
+    <t>3x25</t>
+  </si>
+  <si>
+    <t>13.04.2021 01:05</t>
+  </si>
+  <si>
+    <t>859182400502143132</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400502143132. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>BOHEMIA ENERGY entity s.r.o.</t>
+  </si>
+  <si>
+    <t>distribucnipozadavky@bohemiaenergy.cz</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400502143132</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400502143132 - Antonín Balarin/15.03.1976, Opavská, 66, Dolní Benešov, 747 22.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Gryžboň Jakub
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D02D, Pi 5,175 kW, HDO ANO, KO č. 1114771089 , Antonín Balarin, 732266255</t>
+  </si>
+  <si>
+    <t>Antonín Balarin</t>
+  </si>
+  <si>
+    <t>Opavská, 66, Dolní Benešov, 747 22</t>
+  </si>
+  <si>
+    <t>15.03.1976</t>
+  </si>
+  <si>
+    <t>13.04.2021 01:16</t>
+  </si>
+  <si>
+    <t>859182400610327813</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400610327813. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400610327813</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400610327813 - David Fišer/03.08.1970, Pod Sokolem, 336, Doubravčice, 282 01.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Gryžboň Jakub
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D57D, Pi 3,1 kW, HDO ANO, KO č. 1114782253 , David Fišer, 775261342</t>
+  </si>
+  <si>
+    <t>David Fišer</t>
+  </si>
+  <si>
+    <t>Pod Sokolem, 336, Doubravčice, 282 01</t>
+  </si>
+  <si>
+    <t>03.08.1970</t>
+  </si>
+  <si>
+    <t>13.04.2021 01:26</t>
+  </si>
+  <si>
+    <t>859182400400046009</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400400046009. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400400046009</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400400046009 - Martin Rejha/27.08.1979, Březinova, 2747, Louny, 440 01.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 32,0 A, sazba D45D, Pi 5,46 kW, HDO ANO, KO č. 1114699180 , Martin Rejha, 774226211</t>
+  </si>
+  <si>
+    <t>Martin Rejha</t>
+  </si>
+  <si>
+    <t>Březinova, 2747, Louny, 440 01</t>
+  </si>
+  <si>
+    <t>27.08.1979</t>
+  </si>
+  <si>
+    <t>PE8D45D</t>
+  </si>
+  <si>
+    <t>13.04.2021 01:37</t>
+  </si>
+  <si>
+    <t>859182400608501980</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400608501980. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400608501980</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400608501980 - Jaromír Mrha/24.12.1971, Černíkovice, 7, Chrášťany, 257 56.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D25D, Pi 4,81 kW, HDO ANO, KO č. 1114744271 , Jaromír Mrha, 732109486</t>
+  </si>
+  <si>
+    <t>Jaromír Mrha</t>
+  </si>
+  <si>
+    <t>Černíkovice, 7, Chrášťany, 257 56</t>
+  </si>
+  <si>
+    <t>24.12.1971</t>
+  </si>
+  <si>
+    <t>13.04.2021 01:47</t>
+  </si>
+  <si>
+    <t>859182400509773561</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400509773561. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400509773561</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400509773561 - Lubomír Andrla/10.04.1966, Baška, 501, Baška, 739 01.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Dzurik Ondřej
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D02D, Pi 4,44 kW, HDO ANO, KO č. 1114810193 , Lubomír Andrla, 606621674</t>
+  </si>
+  <si>
+    <t>Lubomír Andrla</t>
+  </si>
+  <si>
+    <t>Baška, 501, Baška, 739 01</t>
+  </si>
+  <si>
+    <t>10.04.1966</t>
+  </si>
+  <si>
+    <t>13.04.2021 01:58</t>
+  </si>
+  <si>
+    <t>Hegerová Eva</t>
+  </si>
+  <si>
+    <t>859182400708221368</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400708221368. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400708221368</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400708221368 - Jiří Bubník/29.08.1977, Bílá Třemešná, 449, Bílá Třemešná, 544 72.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Hegerová Eva
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 25,0 A, sazba D57D, Pi 5,18 kW, HDO ANO, KO č. 1114781114 , Jiří Bubník, 736222931</t>
+  </si>
+  <si>
+    <t>HEGEROVAEVA1</t>
+  </si>
+  <si>
+    <t>Jiří Bubník</t>
+  </si>
+  <si>
+    <t>Bílá Třemešná, 449, Bílá Třemešná, 544 72</t>
+  </si>
+  <si>
+    <t>29.08.1977</t>
+  </si>
+  <si>
+    <t>13.04.2021 02:07</t>
+  </si>
+  <si>
+    <t>859182400505812318</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400505812318. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>innogy Energie, s.r.o.</t>
+  </si>
+  <si>
+    <t>zmenadodavatele@innogy.cz</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400505812318</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400505812318 - Vítězslava Blažková/27.02.1981, Marie Kudeříkové, 226, Křelov-Břuchotín, 783 36.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Hegerová Eva
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 20,0 A, sazba D02D, Pi 4,1 kW, HDO ANO, KO č. 1114782160 , Vítězslava Blažková, 724692633</t>
+  </si>
+  <si>
+    <t>Vítězslava Blažková</t>
+  </si>
+  <si>
+    <t>Marie Kudeříkové, 226, Křelov-Břuchotín, 783 36</t>
+  </si>
+  <si>
+    <t>27.02.1981</t>
+  </si>
+  <si>
+    <t>20,0</t>
+  </si>
+  <si>
+    <t>13.04.2021 02:18</t>
+  </si>
+  <si>
+    <t>859182400504889052</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje (MS) na hladině NN ve stávajícím OM k datu 21.4.2021. EAN 859182400504889052. Žádám o aktualizaci dat v CS OTE. Děkuji.</t>
+  </si>
+  <si>
+    <t>Připojení mikrozdroje EAN 859182400504889052</t>
+  </si>
+  <si>
+    <t>Vážený obchodní partnere, 
+dovolujeme si Vás informovat, že vznikl nový mikrozdroj na hladině NN ve stávajícím OM, EAN 859182400504889052 - Michal Holiš/11.12.1977, Náves, 19, Velký Týnec, 783 72.
+Montáž 4Q elektroměru bude 21.04.2021. Změna typu měření z C na B bude provedena.
+NA TENTO E-MAIL, PROSÍM, NEODPOVÍDEJTE.
+Děkujeme Vám.
+S pozdravem
+Hegerová Eva
+ČEZ Distribuce, a. s.
+Guldenerova 2577/19
+326 00 PLZEŇ
+www.cezdistribuce.cz/dodavatel</t>
+  </si>
+  <si>
+    <t>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 3x 40,0 A, sazba D45D, Pi 6,7 kW, HDO ANO, KO č. 1114794267 , Michal Holiš, 724444404</t>
+  </si>
+  <si>
+    <t>Michal Holiš</t>
+  </si>
+  <si>
+    <t>Náves, 19, Velký Týnec, 783 72</t>
+  </si>
+  <si>
+    <t>11.12.1977</t>
+  </si>
+  <si>
+    <t>40,0</t>
+  </si>
+  <si>
+    <t>13.04.2021 02:29</t>
   </si>
 </sst>
 </file>
@@ -224,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -233,6 +924,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -514,18 +1211,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="4" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -564,7 +1262,7 @@
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -664,6 +1362,1878 @@
         <v>34</v>
       </c>
       <c r="AJ1" s="5"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>1113392241</v>
+      </c>
+      <c r="E2">
+        <v>4121754474</v>
+      </c>
+      <c r="F2">
+        <v>840036</v>
+      </c>
+      <c r="G2">
+        <v>1466451</v>
+      </c>
+      <c r="H2">
+        <v>2021817</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2">
+        <v>44251</v>
+      </c>
+      <c r="L2">
+        <v>70000821</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2">
+        <v>608370855</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2">
+        <v>10892308</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2">
+        <v>4440</v>
+      </c>
+      <c r="AD2">
+        <v>102586526</v>
+      </c>
+      <c r="AE2">
+        <v>1113456446</v>
+      </c>
+      <c r="AF2">
+        <v>20001209</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3">
+        <v>1113392241</v>
+      </c>
+      <c r="E3">
+        <v>4121754474</v>
+      </c>
+      <c r="F3">
+        <v>840036</v>
+      </c>
+      <c r="G3">
+        <v>1466451</v>
+      </c>
+      <c r="H3">
+        <v>2021817</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3">
+        <v>44251</v>
+      </c>
+      <c r="L3">
+        <v>70000821</v>
+      </c>
+      <c r="M3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3">
+        <v>608370855</v>
+      </c>
+      <c r="T3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3">
+        <v>10892308</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3">
+        <v>4440</v>
+      </c>
+      <c r="AD3">
+        <v>102586526</v>
+      </c>
+      <c r="AE3">
+        <v>1113456446</v>
+      </c>
+      <c r="AF3">
+        <v>20001209</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4">
+        <v>1113392241</v>
+      </c>
+      <c r="E4">
+        <v>4121754474</v>
+      </c>
+      <c r="F4">
+        <v>840036</v>
+      </c>
+      <c r="G4">
+        <v>1466451</v>
+      </c>
+      <c r="H4">
+        <v>2021817</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4">
+        <v>44251</v>
+      </c>
+      <c r="L4">
+        <v>70000821</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4">
+        <v>608370855</v>
+      </c>
+      <c r="T4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s">
+        <v>47</v>
+      </c>
+      <c r="X4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4">
+        <v>10892308</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC4">
+        <v>4440</v>
+      </c>
+      <c r="AD4">
+        <v>102586526</v>
+      </c>
+      <c r="AE4">
+        <v>1113456446</v>
+      </c>
+      <c r="AF4">
+        <v>20001209</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>1113392241</v>
+      </c>
+      <c r="E5">
+        <v>4121754474</v>
+      </c>
+      <c r="F5">
+        <v>840036</v>
+      </c>
+      <c r="G5">
+        <v>1466451</v>
+      </c>
+      <c r="H5">
+        <v>2021817</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="8">
+        <v>44251</v>
+      </c>
+      <c r="L5">
+        <v>70000821</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5">
+        <v>608370855</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" t="s">
+        <v>47</v>
+      </c>
+      <c r="X5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA5">
+        <v>10892308</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC5">
+        <v>4440</v>
+      </c>
+      <c r="AD5">
+        <v>102586526</v>
+      </c>
+      <c r="AE5">
+        <v>1113456446</v>
+      </c>
+      <c r="AF5">
+        <v>20001209</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>1113392241</v>
+      </c>
+      <c r="E6">
+        <v>4121754474</v>
+      </c>
+      <c r="F6">
+        <v>840036</v>
+      </c>
+      <c r="G6">
+        <v>1466451</v>
+      </c>
+      <c r="H6">
+        <v>2021817</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="8">
+        <v>44251</v>
+      </c>
+      <c r="L6">
+        <v>70000821</v>
+      </c>
+      <c r="M6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6">
+        <v>608370855</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" t="s">
+        <v>46</v>
+      </c>
+      <c r="V6" t="s">
+        <v>47</v>
+      </c>
+      <c r="X6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA6">
+        <v>10892308</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC6">
+        <v>4440</v>
+      </c>
+      <c r="AD6">
+        <v>102586526</v>
+      </c>
+      <c r="AE6">
+        <v>1113456446</v>
+      </c>
+      <c r="AF6">
+        <v>20001209</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7">
+        <v>1113074378</v>
+      </c>
+      <c r="E7">
+        <v>4121747125</v>
+      </c>
+      <c r="F7">
+        <v>1001246073</v>
+      </c>
+      <c r="G7">
+        <v>10001439953</v>
+      </c>
+      <c r="H7">
+        <v>102491778</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="8">
+        <v>44277</v>
+      </c>
+      <c r="L7">
+        <v>40000821</v>
+      </c>
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" t="s">
+        <v>72</v>
+      </c>
+      <c r="S7">
+        <v>775155495</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" t="s">
+        <v>74</v>
+      </c>
+      <c r="V7" t="s">
+        <v>47</v>
+      </c>
+      <c r="X7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA7">
+        <v>12890759</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7">
+        <v>4400</v>
+      </c>
+      <c r="AD7">
+        <v>102589301</v>
+      </c>
+      <c r="AE7">
+        <v>1114199975</v>
+      </c>
+      <c r="AF7">
+        <v>20004702</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8">
+        <v>1114184179</v>
+      </c>
+      <c r="E8">
+        <v>4121746873</v>
+      </c>
+      <c r="F8">
+        <v>1605661</v>
+      </c>
+      <c r="G8">
+        <v>2760806</v>
+      </c>
+      <c r="H8">
+        <v>4648311</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="8">
+        <v>44277</v>
+      </c>
+      <c r="L8">
+        <v>60000821</v>
+      </c>
+      <c r="M8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O8" t="s">
+        <v>83</v>
+      </c>
+      <c r="P8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" t="s">
+        <v>86</v>
+      </c>
+      <c r="S8">
+        <v>739306042</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="U8" t="s">
+        <v>88</v>
+      </c>
+      <c r="V8" t="s">
+        <v>47</v>
+      </c>
+      <c r="X8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA8">
+        <v>11172340</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC8">
+        <v>8250</v>
+      </c>
+      <c r="AD8">
+        <v>102589304</v>
+      </c>
+      <c r="AE8">
+        <v>1114201746</v>
+      </c>
+      <c r="AF8">
+        <v>20004703</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9">
+        <v>1114734978</v>
+      </c>
+      <c r="E9">
+        <v>4121755845</v>
+      </c>
+      <c r="F9">
+        <v>1000044229</v>
+      </c>
+      <c r="G9">
+        <v>10000058854</v>
+      </c>
+      <c r="H9">
+        <v>100115550</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="8">
+        <v>44306</v>
+      </c>
+      <c r="L9">
+        <v>70000821</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" t="s">
+        <v>95</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" t="s">
+        <v>96</v>
+      </c>
+      <c r="S9">
+        <v>775077382</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="U9" t="s">
+        <v>98</v>
+      </c>
+      <c r="V9" t="s">
+        <v>47</v>
+      </c>
+      <c r="X9" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA9">
+        <v>10742913</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC9">
+        <v>5520</v>
+      </c>
+      <c r="AD9">
+        <v>102592454</v>
+      </c>
+      <c r="AE9">
+        <v>1114799936</v>
+      </c>
+      <c r="AF9">
+        <v>20007403</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10">
+        <v>1114733390</v>
+      </c>
+      <c r="E10">
+        <v>4121724393</v>
+      </c>
+      <c r="F10">
+        <v>2319942</v>
+      </c>
+      <c r="G10">
+        <v>3903890</v>
+      </c>
+      <c r="H10">
+        <v>5564267</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K10" s="8">
+        <v>44302</v>
+      </c>
+      <c r="L10">
+        <v>50000821</v>
+      </c>
+      <c r="M10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" t="s">
+        <v>107</v>
+      </c>
+      <c r="O10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10">
+        <v>739054589</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="U10" t="s">
+        <v>111</v>
+      </c>
+      <c r="V10" t="s">
+        <v>47</v>
+      </c>
+      <c r="X10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA10">
+        <v>13650293</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC10">
+        <v>2580</v>
+      </c>
+      <c r="AD10">
+        <v>102592456</v>
+      </c>
+      <c r="AE10">
+        <v>1114802028</v>
+      </c>
+      <c r="AF10">
+        <v>20007404</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11">
+        <v>1114769081</v>
+      </c>
+      <c r="E11">
+        <v>4121744436</v>
+      </c>
+      <c r="F11">
+        <v>1683217</v>
+      </c>
+      <c r="G11">
+        <v>2845710</v>
+      </c>
+      <c r="H11">
+        <v>3866175</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="8">
+        <v>44306</v>
+      </c>
+      <c r="L11">
+        <v>60000821</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" t="s">
+        <v>118</v>
+      </c>
+      <c r="P11" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>120</v>
+      </c>
+      <c r="R11" t="s">
+        <v>121</v>
+      </c>
+      <c r="S11">
+        <v>603432156</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="U11" t="s">
+        <v>123</v>
+      </c>
+      <c r="V11" t="s">
+        <v>124</v>
+      </c>
+      <c r="X11" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA11" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC11">
+        <v>4.62</v>
+      </c>
+      <c r="AD11">
+        <v>102592830</v>
+      </c>
+      <c r="AE11">
+        <v>1114853007</v>
+      </c>
+      <c r="AF11">
+        <v>20007317</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12">
+        <v>1114771089</v>
+      </c>
+      <c r="E12">
+        <v>4121760018</v>
+      </c>
+      <c r="F12">
+        <v>2018254</v>
+      </c>
+      <c r="G12">
+        <v>3620721</v>
+      </c>
+      <c r="H12">
+        <v>5025009</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L12">
+        <v>50000821</v>
+      </c>
+      <c r="M12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" t="s">
+        <v>132</v>
+      </c>
+      <c r="P12" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12" t="s">
+        <v>135</v>
+      </c>
+      <c r="S12">
+        <v>732266255</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="U12" t="s">
+        <v>137</v>
+      </c>
+      <c r="V12" t="s">
+        <v>124</v>
+      </c>
+      <c r="X12" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA12">
+        <v>14135251</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC12">
+        <v>5175</v>
+      </c>
+      <c r="AD12">
+        <v>102592832</v>
+      </c>
+      <c r="AE12">
+        <v>1114853707</v>
+      </c>
+      <c r="AF12">
+        <v>20007318</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13">
+        <v>1114782253</v>
+      </c>
+      <c r="E13">
+        <v>4121672808</v>
+      </c>
+      <c r="F13">
+        <v>1001257898</v>
+      </c>
+      <c r="G13">
+        <v>10001460549</v>
+      </c>
+      <c r="H13">
+        <v>102503714</v>
+      </c>
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L13">
+        <v>60000821</v>
+      </c>
+      <c r="M13" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" t="s">
+        <v>82</v>
+      </c>
+      <c r="O13" t="s">
+        <v>143</v>
+      </c>
+      <c r="P13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>71</v>
+      </c>
+      <c r="R13" t="s">
+        <v>144</v>
+      </c>
+      <c r="S13">
+        <v>775261342</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="U13" t="s">
+        <v>146</v>
+      </c>
+      <c r="V13" t="s">
+        <v>124</v>
+      </c>
+      <c r="X13" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA13">
+        <v>13821711</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC13">
+        <v>3100</v>
+      </c>
+      <c r="AD13">
+        <v>102592833</v>
+      </c>
+      <c r="AE13">
+        <v>1114854029</v>
+      </c>
+      <c r="AF13">
+        <v>20007319</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14">
+        <v>1114699180</v>
+      </c>
+      <c r="E14">
+        <v>4121772353</v>
+      </c>
+      <c r="F14">
+        <v>3530940</v>
+      </c>
+      <c r="G14">
+        <v>4838913</v>
+      </c>
+      <c r="H14">
+        <v>7975155</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L14">
+        <v>40000821</v>
+      </c>
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" t="s">
+        <v>152</v>
+      </c>
+      <c r="P14" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>134</v>
+      </c>
+      <c r="R14" t="s">
+        <v>153</v>
+      </c>
+      <c r="S14">
+        <v>774226211</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="U14" t="s">
+        <v>155</v>
+      </c>
+      <c r="V14" t="s">
+        <v>47</v>
+      </c>
+      <c r="X14" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA14">
+        <v>12885149</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC14">
+        <v>5460</v>
+      </c>
+      <c r="AD14">
+        <v>102592834</v>
+      </c>
+      <c r="AE14">
+        <v>1114854268</v>
+      </c>
+      <c r="AF14">
+        <v>20007321</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15">
+        <v>1114744271</v>
+      </c>
+      <c r="E15">
+        <v>4121767836</v>
+      </c>
+      <c r="F15">
+        <v>1000054423</v>
+      </c>
+      <c r="G15">
+        <v>10000072020</v>
+      </c>
+      <c r="H15">
+        <v>100143436</v>
+      </c>
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L15">
+        <v>60000821</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" t="s">
+        <v>82</v>
+      </c>
+      <c r="O15" t="s">
+        <v>162</v>
+      </c>
+      <c r="P15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>71</v>
+      </c>
+      <c r="R15" t="s">
+        <v>163</v>
+      </c>
+      <c r="S15">
+        <v>732109486</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="U15" t="s">
+        <v>165</v>
+      </c>
+      <c r="V15" t="s">
+        <v>47</v>
+      </c>
+      <c r="X15" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA15">
+        <v>13207493</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC15">
+        <v>4810</v>
+      </c>
+      <c r="AD15">
+        <v>102592835</v>
+      </c>
+      <c r="AE15">
+        <v>1114854554</v>
+      </c>
+      <c r="AF15">
+        <v>20007322</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16">
+        <v>1114810193</v>
+      </c>
+      <c r="E16">
+        <v>4121738817</v>
+      </c>
+      <c r="F16">
+        <v>2677671</v>
+      </c>
+      <c r="G16">
+        <v>4281130</v>
+      </c>
+      <c r="H16">
+        <v>6304620</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L16">
+        <v>50000821</v>
+      </c>
+      <c r="M16" t="s">
+        <v>39</v>
+      </c>
+      <c r="N16" t="s">
+        <v>107</v>
+      </c>
+      <c r="O16" t="s">
+        <v>171</v>
+      </c>
+      <c r="P16" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>71</v>
+      </c>
+      <c r="R16" t="s">
+        <v>172</v>
+      </c>
+      <c r="S16">
+        <v>606621674</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="U16" t="s">
+        <v>174</v>
+      </c>
+      <c r="V16" t="s">
+        <v>47</v>
+      </c>
+      <c r="X16" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA16">
+        <v>12418674</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC16">
+        <v>4440</v>
+      </c>
+      <c r="AD16">
+        <v>102592836</v>
+      </c>
+      <c r="AE16">
+        <v>1114854890</v>
+      </c>
+      <c r="AF16">
+        <v>20007323</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17">
+        <v>1114781114</v>
+      </c>
+      <c r="E17">
+        <v>4121774738</v>
+      </c>
+      <c r="F17">
+        <v>1001263289</v>
+      </c>
+      <c r="G17">
+        <v>10001474656</v>
+      </c>
+      <c r="H17">
+        <v>102509500</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L17">
+        <v>70000821</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" t="s">
+        <v>181</v>
+      </c>
+      <c r="P17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>71</v>
+      </c>
+      <c r="R17" t="s">
+        <v>182</v>
+      </c>
+      <c r="S17">
+        <v>736222931</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="U17" t="s">
+        <v>184</v>
+      </c>
+      <c r="V17" t="s">
+        <v>185</v>
+      </c>
+      <c r="X17" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA17">
+        <v>20087837</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC17">
+        <v>5180</v>
+      </c>
+      <c r="AD17">
+        <v>102592837</v>
+      </c>
+      <c r="AE17">
+        <v>1114855093</v>
+      </c>
+      <c r="AF17">
+        <v>20007324</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18">
+        <v>1114782160</v>
+      </c>
+      <c r="E18">
+        <v>4121745881</v>
+      </c>
+      <c r="F18">
+        <v>2589781</v>
+      </c>
+      <c r="G18">
+        <v>4147788</v>
+      </c>
+      <c r="H18">
+        <v>6059682</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L18">
+        <v>50000821</v>
+      </c>
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" t="s">
+        <v>191</v>
+      </c>
+      <c r="P18" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>193</v>
+      </c>
+      <c r="R18" t="s">
+        <v>194</v>
+      </c>
+      <c r="S18">
+        <v>724692633</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="U18" t="s">
+        <v>196</v>
+      </c>
+      <c r="V18" t="s">
+        <v>185</v>
+      </c>
+      <c r="X18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA18">
+        <v>13147585</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC18">
+        <v>4100</v>
+      </c>
+      <c r="AD18">
+        <v>102592838</v>
+      </c>
+      <c r="AE18">
+        <v>1114855460</v>
+      </c>
+      <c r="AF18">
+        <v>20007325</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19">
+        <v>1114794267</v>
+      </c>
+      <c r="E19">
+        <v>4121720023</v>
+      </c>
+      <c r="F19">
+        <v>2580696</v>
+      </c>
+      <c r="G19">
+        <v>4176436</v>
+      </c>
+      <c r="H19">
+        <v>5929264</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="8">
+        <v>44307</v>
+      </c>
+      <c r="L19">
+        <v>50000821</v>
+      </c>
+      <c r="M19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O19" t="s">
+        <v>203</v>
+      </c>
+      <c r="P19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R19" t="s">
+        <v>204</v>
+      </c>
+      <c r="S19">
+        <v>724444404</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="U19" t="s">
+        <v>206</v>
+      </c>
+      <c r="V19" t="s">
+        <v>185</v>
+      </c>
+      <c r="X19" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA19">
+        <v>13108780</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC19">
+        <v>6700</v>
+      </c>
+      <c r="AD19">
+        <v>102592840</v>
+      </c>
+      <c r="AE19">
+        <v>1114855636</v>
+      </c>
+      <c r="AF19">
+        <v>20007326</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -672,25 +3242,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007F6D915BEE4E844FB48C3AE514D89089" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="d4ba2a939a563b1bbfc9e4824525ecf9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f7ae4a0-3828-4c27-918b-e30655340dac" xmlns:ns3="15216789-4c43-43b8-8f31-b3ff70bf4c88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c2e2fc7f2dd948a6f921154beffe86e" ns2:_="" ns3:_="">
-    <xsd:import namespace="6f7ae4a0-3828-4c27-918b-e30655340dac"/>
-    <xsd:import namespace="15216789-4c43-43b8-8f31-b3ff70bf4c88"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E6E84BFBB2A2F148AAA86E0A86F7A4AD" ma:contentTypeVersion="11" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="d9c20761254319cb78414ea2f386b971">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6232a9f2-e1b2-483f-a925-f104c4093263" xmlns:ns3="26879c1c-1a95-4f1c-8e74-9e0c0f404514" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba2bdc32c12534def7293fb085105b60" ns2:_="" ns3:_="">
+    <xsd:import namespace="6232a9f2-e1b2-483f-a925-f104c4093263"/>
+    <xsd:import namespace="26879c1c-1a95-4f1c-8e74-9e0c0f404514"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -703,10 +3258,11 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -714,7 +3270,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6f7ae4a0-3828-4c27-918b-e30655340dac" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6232a9f2-e1b2-483f-a925-f104c4093263" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -749,21 +3305,28 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="15216789-4c43-43b8-8f31-b3ff70bf4c88" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="26879c1c-1a95-4f1c-8e74-9e0c0f404514" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Sdílí se s" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Sdílí se s" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -782,7 +3345,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Sdílené s podrobnostmi" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Sdílené s podrobnostmi" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -889,7 +3452,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981294E8-3DCA-4B64-9751-022312752898}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -897,30 +3479,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEAB0EC7-3D52-4496-A75B-1E8C2D12B388}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42B4D896-6DC2-4F3D-AD63-C8A6A3E9E773}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6f7ae4a0-3828-4c27-918b-e30655340dac"/>
-    <ds:schemaRef ds:uri="15216789-4c43-43b8-8f31-b3ff70bf4c88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>